<commit_message>
Added a PolynomialCalculator page.
</commit_message>
<xml_diff>
--- a/CalculatorApp/CalculatorApp/Resources/scheme.xlsx
+++ b/CalculatorApp/CalculatorApp/Resources/scheme.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bobi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\CalculatorApp\CalculatorApp\CalculatorApp\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BasicCalculator" sheetId="1" r:id="rId1"/>
+    <sheet name="PolynomialCalculator" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -125,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>=</t>
   </si>
@@ -182,6 +183,18 @@
   </si>
   <si>
     <t>√</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>simplified</t>
+  </si>
+  <si>
+    <t>range</t>
   </si>
 </sst>
 </file>
@@ -241,14 +254,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -257,6 +264,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -540,130 +556,130 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="I1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I1" s="4">
+      <c r="I1" s="6">
         <v>22.5</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
     </row>
     <row r="2" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
     </row>
     <row r="3" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="1">
         <v>7</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="1">
         <v>8</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="1">
         <v>9</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="1">
         <v>4</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="1">
         <v>5</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="1">
         <v>6</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="1">
         <v>1</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="1">
         <v>2</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="1">
         <v>3</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="1">
         <v>0</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M8" s="2"/>
+      <c r="M8" s="5"/>
     </row>
     <row r="9" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -692,4 +708,93 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="I1:M28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+    </row>
+    <row r="2" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+    </row>
+    <row r="4" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="9:13" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="I2:M2"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="I4:M4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>